<commit_message>
モジュール名変更　broccoli-html-editor--table-field -> broccoli-field-table
</commit_message>
<xml_diff>
--- a/tests/testdata/htdocs/editpage/index_files/guieditor.ignore/resources/9d8d3961c3c1cf3725055d908e4be33a/bin.xlsx
+++ b/tests/testdata/htdocs/editpage/index_files/guieditor.ignore/resources/9d8d3961c3c1cf3725055d908e4be33a/bin.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="tab1" sheetId="1" r:id="rId4"/>
+    <sheet name="tab1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
   <si>
     <t>A1</t>
   </si>
@@ -94,12 +102,6 @@
     <t>B6</t>
   </si>
   <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
     <t>E6</t>
   </si>
   <si>
@@ -109,12 +111,6 @@
     <t>B7</t>
   </si>
   <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
     <t>E7</t>
   </si>
   <si>
@@ -124,12 +120,6 @@
     <t>B8</t>
   </si>
   <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
     <t>E8</t>
   </si>
   <si>
@@ -139,12 +129,6 @@
     <t>B9</t>
   </si>
   <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>D9</t>
-  </si>
-  <si>
     <t>E9</t>
   </si>
   <si>
@@ -154,12 +138,6 @@
     <t>B10</t>
   </si>
   <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>D10</t>
-  </si>
-  <si>
     <t>E10</t>
   </si>
   <si>
@@ -169,12 +147,6 @@
     <t>B11</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
     <t>E11</t>
   </si>
   <si>
@@ -182,12 +154,6 @@
   </si>
   <si>
     <t>B12</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>D12</t>
   </si>
   <si>
     <t>E12</t>
@@ -286,11 +252,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -299,22 +262,28 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="ヒラギノ角ゴ ProN W3"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="メイリオ"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="5">
@@ -367,54 +336,108 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffcccccc"/>
-      <rgbColor rgb="ffdddddd"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -606,7 +629,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -615,7 +638,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -624,7 +647,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -633,7 +656,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -642,7 +665,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -651,7 +674,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -763,8 +786,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -772,14 +795,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -798,7 +821,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -806,7 +829,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -834,7 +857,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -860,7 +883,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -886,7 +909,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -912,7 +935,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -938,7 +961,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -964,7 +987,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -990,7 +1013,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1016,7 +1039,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1042,7 +1065,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1055,9 +1078,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1073,7 +1102,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1092,7 +1121,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1118,7 +1147,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1144,7 +1173,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1170,7 +1199,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1196,7 +1225,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1222,7 +1251,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1248,7 +1277,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1274,7 +1303,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1300,7 +1329,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1326,7 +1355,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1339,9 +1368,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1354,7 +1389,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1373,7 +1408,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1403,7 +1438,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1429,7 +1464,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1455,7 +1490,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1481,7 +1516,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1507,7 +1542,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1533,7 +1568,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1559,7 +1594,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1585,7 +1620,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1611,7 +1646,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1624,343 +1659,358 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="7.625" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5312" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5469" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.0469" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26562" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.25" style="1" customWidth="1"/>
     <col min="6" max="256" width="7.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="19" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="19" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:5" ht="19" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="19" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" spans="1:5" ht="19" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s" s="4">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" ht="19" customHeight="1">
-      <c r="A4" t="s" s="4">
+    <row r="4" spans="1:5" ht="19" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s" s="4">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s" s="4">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" ht="19" customHeight="1">
-      <c r="A5" t="s" s="4">
+    <row r="5" spans="1:5" ht="19" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s" s="4">
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s" s="4">
+      <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" ht="19" customHeight="1">
-      <c r="A6" t="s" s="4">
+    <row r="6" spans="1:5" ht="19" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s" s="4">
+    </row>
+    <row r="7" spans="1:5" ht="19" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s" s="4">
+      <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" ht="19" customHeight="1">
-      <c r="A7" t="s" s="4">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s" s="4">
+    <row r="8" spans="1:5" ht="19" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s" s="4">
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s" s="4">
+    </row>
+    <row r="9" spans="1:5" ht="19" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" ht="19" customHeight="1">
-      <c r="A8" t="s" s="4">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s" s="4">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s" s="4">
+    <row r="10" spans="1:5" ht="19" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D8" t="s" s="4">
+      <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="s" s="4">
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" ht="19" customHeight="1">
-      <c r="A9" t="s" s="4">
+    <row r="11" spans="1:5" ht="19" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s" s="4">
+      <c r="B11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s" s="4">
+      <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D9" t="s" s="4">
+    </row>
+    <row r="12" spans="1:5" ht="19" customHeight="1">
+      <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E9" t="s" s="4">
+      <c r="B12" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="10" ht="19" customHeight="1">
-      <c r="A10" t="s" s="4">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s" s="4">
+    <row r="13" spans="1:5" ht="19" customHeight="1">
+      <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C10" t="s" s="4">
+      <c r="B13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D10" t="s" s="4">
+      <c r="C13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E10" t="s" s="4">
+      <c r="D13" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="E13" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="11" ht="19" customHeight="1">
-      <c r="A11" t="s" s="4">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s" s="4">
+    <row r="14" spans="1:5" ht="19" customHeight="1">
+      <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s" s="4">
+      <c r="B14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D11" t="s" s="4">
+      <c r="C14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E11" t="s" s="4">
+      <c r="D14" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="E14" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="12" ht="19" customHeight="1">
-      <c r="A12" t="s" s="4">
-        <v>55</v>
-      </c>
-      <c r="B12" t="s" s="4">
+    <row r="15" spans="1:5" ht="19" customHeight="1">
+      <c r="A15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C12" t="s" s="4">
+      <c r="B15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D12" t="s" s="4">
+      <c r="C15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E12" t="s" s="4">
+      <c r="D15" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="E15" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="13" ht="19" customHeight="1">
-      <c r="A13" t="s" s="4">
-        <v>60</v>
-      </c>
-      <c r="B13" t="s" s="4">
+    <row r="16" spans="1:5" ht="19" customHeight="1">
+      <c r="A16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C13" t="s" s="4">
+      <c r="B16" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D13" t="s" s="4">
+      <c r="C16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E13" t="s" s="4">
+      <c r="D16" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="E16" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="14" ht="19" customHeight="1">
-      <c r="A14" t="s" s="4">
-        <v>65</v>
-      </c>
-      <c r="B14" t="s" s="4">
+    <row r="17" spans="1:5" ht="19" customHeight="1">
+      <c r="A17" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C14" t="s" s="4">
+      <c r="B17" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D14" t="s" s="4">
+      <c r="C17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E14" t="s" s="4">
+      <c r="D17" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="E17" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="15" ht="19" customHeight="1">
-      <c r="A15" t="s" s="4">
-        <v>70</v>
-      </c>
-      <c r="B15" t="s" s="4">
+    <row r="18" spans="1:5" ht="19" customHeight="1">
+      <c r="A18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C15" t="s" s="4">
+      <c r="B18" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D15" t="s" s="4">
+      <c r="C18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E15" t="s" s="4">
+      <c r="D18" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" ht="19" customHeight="1">
-      <c r="A16" t="s" s="4">
+      <c r="E18" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B16" t="s" s="4">
-        <v>76</v>
-      </c>
-      <c r="C16" t="s" s="4">
-        <v>77</v>
-      </c>
-      <c r="D16" t="s" s="4">
-        <v>78</v>
-      </c>
-      <c r="E16" t="s" s="4">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" ht="19" customHeight="1">
-      <c r="A17" t="s" s="4">
-        <v>80</v>
-      </c>
-      <c r="B17" t="s" s="4">
-        <v>81</v>
-      </c>
-      <c r="C17" t="s" s="4">
-        <v>82</v>
-      </c>
-      <c r="D17" t="s" s="4">
-        <v>83</v>
-      </c>
-      <c r="E17" t="s" s="4">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" ht="19" customHeight="1">
-      <c r="A18" t="s" s="4">
-        <v>85</v>
-      </c>
-      <c r="B18" t="s" s="4">
-        <v>86</v>
-      </c>
-      <c r="C18" t="s" s="4">
-        <v>87</v>
-      </c>
-      <c r="D18" t="s" s="4">
-        <v>88</v>
-      </c>
-      <c r="E18" t="s" s="4">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>